<commit_message>
added rear inner tyre
</commit_message>
<xml_diff>
--- a/tkph_tracking.xlsx
+++ b/tkph_tracking.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1313,11 +1313,7 @@
           <t>2024-12-13 03:13:35</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
           <t>rear-right</t>
@@ -1328,6 +1324,29 @@
       </c>
       <c r="E43" t="n">
         <v>3888</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-12-13 04:33:38</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>rear-left-outer</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>1920</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1920</v>
       </c>
     </row>
   </sheetData>

</xml_diff>